<commit_message>
Included densification in VSwellingUC
</commit_message>
<xml_diff>
--- a/tests/materials/VSwellingUC/VswellingUC.xlsx
+++ b/tests/materials/VSwellingUC/VswellingUC.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-11060" yWindow="-18000" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-11060" yWindow="-18000" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="solid" sheetId="1" r:id="rId1"/>
     <sheet name="gas" sheetId="2" r:id="rId2"/>
+    <sheet name="densification" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>DV/v</t>
   </si>
@@ -122,6 +123,27 @@
   </si>
   <si>
     <t>Step</t>
+  </si>
+  <si>
+    <t>total dens</t>
+  </si>
+  <si>
+    <t>Bmax</t>
+  </si>
+  <si>
+    <t>dens</t>
+  </si>
+  <si>
+    <t>BUCK vol</t>
+  </si>
+  <si>
+    <t>EXCEL vol</t>
+  </si>
+  <si>
+    <t>% Diff</t>
+  </si>
+  <si>
+    <t>3=</t>
   </si>
 </sst>
 </file>
@@ -133,8 +155,8 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0000E+00"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
-    <numFmt numFmtId="171" formatCode="0.000000E+00"/>
-    <numFmt numFmtId="173" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="169" formatCode="0.00000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -186,9 +208,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="220">
+  <cellStyleXfs count="246">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -418,10 +466,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="220">
+  <cellStyles count="246">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -531,6 +579,19 @@
     <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -640,6 +701,19 @@
     <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1164,7 +1238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K24" sqref="K24:Q35"/>
     </sheetView>
   </sheetViews>
@@ -1313,19 +1387,19 @@
         <v>1.0176430000000001</v>
       </c>
       <c r="H13" s="8">
-        <f>$B$2*($E13*100-$B$3)</f>
+        <f t="shared" ref="H13:H19" si="0">$B$2*($E13*100-$B$3)</f>
         <v>6.8939839999999988E-2</v>
       </c>
       <c r="I13" s="5">
-        <f>$B$5*($E13*100-$B$6)</f>
+        <f t="shared" ref="I13:I19" si="1">$B$5*($E13*100-$B$6)</f>
         <v>1.7313388099999998</v>
       </c>
       <c r="J13" s="4">
-        <f>$I13-$B$7*($E13*100-$B$6)*($B13-$D$10)</f>
+        <f t="shared" ref="J13:J19" si="2">$I13-$B$7*($E13*100-$B$6)*($B13-$D$10)</f>
         <v>1.2205373736500003</v>
       </c>
       <c r="K13" s="5">
-        <f>$I13-$B$8*($E13*100-$B$6)*($B13-$D$10)</f>
+        <f t="shared" ref="K13:K19" si="3">$I13-$B$8*($E13*100-$B$6)*($B13-$D$10)</f>
         <v>-2.2415612504999958</v>
       </c>
       <c r="L13" s="9">
@@ -1333,7 +1407,7 @@
         <v>0.47411200000000009</v>
       </c>
       <c r="M13" s="3">
-        <f t="shared" ref="M13:M18" si="0">0.5-0.025*(C13-D13)</f>
+        <f t="shared" ref="M13:M18" si="4">0.5-0.025*(C13-D13)</f>
         <v>-0.147199999999998</v>
       </c>
       <c r="N13" s="8">
@@ -1369,27 +1443,27 @@
         <v>1.0769169999999999</v>
       </c>
       <c r="H14" s="8">
-        <f>$B$2*($E14*100-$B$3)</f>
+        <f t="shared" si="0"/>
         <v>0.18587967999999999</v>
       </c>
       <c r="I14" s="5">
-        <f>$B$5*($E14*100-$B$6)</f>
+        <f t="shared" si="1"/>
         <v>3.9714676199999994</v>
       </c>
       <c r="J14" s="4">
-        <f>$I14-$B$7*($E14*100-$B$6)*($B14-$D$10)</f>
+        <f t="shared" si="2"/>
         <v>3.8765994301799998</v>
       </c>
       <c r="K14" s="5">
-        <f>$I14-$B$8*($E14*100-$B$6)*($B14-$D$10)</f>
+        <f t="shared" si="3"/>
         <v>3.2336039214000003</v>
       </c>
       <c r="L14" s="7">
-        <f t="shared" ref="L14:L19" si="1">0.5-0.001*(C14-D14)</f>
+        <f t="shared" ref="L14:L19" si="5">0.5-0.001*(C14-D14)</f>
         <v>0.62490299999999999</v>
       </c>
       <c r="M14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3.6225750000000008</v>
       </c>
       <c r="N14" s="8">
@@ -1425,27 +1499,27 @@
         <v>1.175767</v>
       </c>
       <c r="H15" s="8">
-        <f>$B$2*($E15*100-$B$3)</f>
+        <f t="shared" si="0"/>
         <v>0.30281952000000001</v>
       </c>
       <c r="I15" s="5">
-        <f>$B$5*($E15*100-$B$6)</f>
+        <f t="shared" si="1"/>
         <v>6.2115964300000002</v>
       </c>
       <c r="J15" s="4">
-        <f>$I15-$B$7*($E15*100-$B$6)*($B15-$D$10)</f>
+        <f t="shared" si="2"/>
         <v>6.9361827001480023</v>
       </c>
       <c r="K15" s="5">
-        <f>$I15-$B$8*($E15*100-$B$6)*($B15-$D$10)</f>
+        <f t="shared" si="3"/>
         <v>11.847267420040016</v>
       </c>
       <c r="L15" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.69616499999999992</v>
       </c>
       <c r="M15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>5.4041249999999996</v>
       </c>
       <c r="N15" s="8">
@@ -1481,31 +1555,31 @@
         <v>1.292019</v>
       </c>
       <c r="H16" s="8">
-        <f>$B$2*($E16*100-$B$3)</f>
+        <f t="shared" si="0"/>
         <v>0.41975935999999997</v>
       </c>
       <c r="I16" s="5">
-        <f>$B$5*($E16*100-$B$6)</f>
+        <f t="shared" si="1"/>
         <v>8.4517252399999983</v>
       </c>
       <c r="J16" s="4">
-        <f>$I16-$B$7*($E16*100-$B$6)*($B16-$D$10)</f>
+        <f t="shared" si="2"/>
         <v>10.221533050232001</v>
       </c>
       <c r="K16" s="5">
-        <f>$I16-$B$8*($E16*100-$B$6)*($B16-$D$10)</f>
+        <f t="shared" si="3"/>
         <v>22.216897097360018</v>
       </c>
       <c r="L16" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.74089149999999993</v>
       </c>
       <c r="M16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>6.5222874999999991</v>
       </c>
       <c r="N16" s="8">
-        <f t="shared" ref="N16:N17" si="2">(H16+K16+M16)/100+1</f>
+        <f t="shared" ref="N16:N17" si="6">(H16+K16+M16)/100+1</f>
         <v>1.2915894395736003</v>
       </c>
       <c r="O16" s="7">
@@ -1537,31 +1611,31 @@
         <v>1.417082</v>
       </c>
       <c r="H17" s="8">
-        <f>$B$2*($E17*100-$B$3)</f>
+        <f t="shared" si="0"/>
         <v>0.53669920000000004</v>
       </c>
       <c r="I17" s="5">
-        <f>$B$5*($E17*100-$B$6)</f>
+        <f t="shared" si="1"/>
         <v>10.691854050000002</v>
       </c>
       <c r="J17" s="4">
-        <f>$I17-$B$7*($E17*100-$B$6)*($B17-$D$10)</f>
+        <f t="shared" si="2"/>
         <v>13.661287152060005</v>
       </c>
       <c r="K17" s="5">
-        <f>$I17-$B$8*($E17*100-$B$6)*($B17-$D$10)</f>
+        <f t="shared" si="3"/>
         <v>33.787444843800031</v>
       </c>
       <c r="L17" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.77273930000000002</v>
       </c>
       <c r="M17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7.3184824999999991</v>
       </c>
       <c r="N17" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.4164262654380004</v>
       </c>
       <c r="O17" s="7">
@@ -1593,27 +1667,27 @@
         <v>1.4430000000000001</v>
       </c>
       <c r="H18" s="8">
-        <f>$B$2*($E18*100-$B$3)</f>
+        <f t="shared" si="0"/>
         <v>0.65363904000000006</v>
       </c>
       <c r="I18" s="5">
-        <f>$B$5*($E18*100-$B$6)</f>
+        <f t="shared" si="1"/>
         <v>12.931982860000002</v>
       </c>
       <c r="J18" s="4">
-        <f>$I18-$B$7*($E18*100-$B$6)*($B18-$D$10)</f>
+        <f t="shared" si="2"/>
         <v>17.217182082207998</v>
       </c>
       <c r="K18" s="5">
-        <f>$I18-$B$8*($E18*100-$B$6)*($B18-$D$10)</f>
+        <f t="shared" si="3"/>
         <v>46.261310143839992</v>
       </c>
       <c r="L18" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.79711529999999997</v>
       </c>
       <c r="M18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7.9278825000000017</v>
       </c>
       <c r="N18" s="8"/>
@@ -1642,23 +1716,23 @@
         <v>1.4430000000000001</v>
       </c>
       <c r="H19" s="8">
-        <f>$B$2*($E19*100-$B$3)</f>
+        <f t="shared" si="0"/>
         <v>0.77057887999999997</v>
       </c>
       <c r="I19" s="5">
-        <f>$B$5*($E19*100-$B$6)</f>
+        <f t="shared" si="1"/>
         <v>15.17211167</v>
       </c>
       <c r="J19" s="4">
-        <f>$I19-$B$7*($E19*100-$B$6)*($B19-$D$10)</f>
+        <f t="shared" si="2"/>
         <v>20.865559189352002</v>
       </c>
       <c r="K19" s="5">
-        <f>$I19-$B$8*($E19*100-$B$6)*($B19-$D$10)</f>
+        <f t="shared" si="3"/>
         <v>59.454481264960016</v>
       </c>
       <c r="L19" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.81666879999999997</v>
       </c>
       <c r="M19" s="3">
@@ -1976,4 +2050,251 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="4" spans="3:9">
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4">
+        <v>-3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9">
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9">
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9">
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
+      <c r="G8" s="7">
+        <f>$G$4*(1-EXP(-E8/$G$5))</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <f>(1+G8)</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="7">
+        <f>ABS(F8-H8)/H8*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9">
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9" s="7">
+        <v>3.6543700000000001E-3</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.98449540000000002</v>
+      </c>
+      <c r="G9" s="7">
+        <f>$G$4*(1-EXP(-E9/$G$5))</f>
+        <v>-1.550872761216435E-2</v>
+      </c>
+      <c r="H9" s="7">
+        <f>(1+G9)</f>
+        <v>0.98449127238783563</v>
+      </c>
+      <c r="I9" s="7">
+        <f>ABS(F9-H9)/H9*100</f>
+        <v>4.1926345922639255E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9">
+      <c r="D10">
+        <v>30</v>
+      </c>
+      <c r="E10" s="7">
+        <v>7.3087400000000002E-3</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.97606199999999999</v>
+      </c>
+      <c r="G10" s="7">
+        <f>$G$4*(1-EXP(-E10/$G$5))</f>
+        <v>-2.3943318984672553E-2</v>
+      </c>
+      <c r="H10" s="7">
+        <f>(1+G10)</f>
+        <v>0.9760566810153275</v>
+      </c>
+      <c r="I10" s="7">
+        <f>ABS(F10-H10)/H10*100</f>
+        <v>5.4494629010208746E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9">
+      <c r="D11">
+        <v>40</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1.096311E-2</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.97147510000000004</v>
+      </c>
+      <c r="G11" s="7">
+        <f>$G$4*(1-EXP(-E11/$G$5))</f>
+        <v>-2.8530563883176607E-2</v>
+      </c>
+      <c r="H11" s="7">
+        <f>(1+G11)</f>
+        <v>0.97146943611682335</v>
+      </c>
+      <c r="I11" s="7">
+        <f>ABS(F11-H11)/H11*100</f>
+        <v>5.8302227184082274E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9">
+      <c r="D12">
+        <v>50</v>
+      </c>
+      <c r="E12" s="7">
+        <v>1.461748E-2</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.96898039999999996</v>
+      </c>
+      <c r="G12" s="7">
+        <f>$G$4*(1-EXP(-E12/$G$5))</f>
+        <v>-3.1025387263410368E-2</v>
+      </c>
+      <c r="H12" s="7">
+        <f>(1+G12)</f>
+        <v>0.96897461273658958</v>
+      </c>
+      <c r="I12" s="7">
+        <f>ABS(F12-H12)/H12*100</f>
+        <v>5.9725645381352962E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9">
+      <c r="D13">
+        <v>60</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1.8271849999999999E-2</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0.96762360000000003</v>
+      </c>
+      <c r="G13" s="7">
+        <f>$G$4*(1-EXP(-E13/$G$5))</f>
+        <v>-3.2382224283511646E-2</v>
+      </c>
+      <c r="H13" s="7">
+        <f>(1+G13)</f>
+        <v>0.96761777571648833</v>
+      </c>
+      <c r="I13" s="7">
+        <f>ABS(F13-H13)/H13*100</f>
+        <v>6.0191985491265252E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="7:10">
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="7:10">
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="7:10">
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="7:10">
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="7:10">
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="7:10">
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="7:10">
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="7:10">
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added additional tests to VSwellingUC
</commit_message>
<xml_diff>
--- a/tests/materials/VSwellingUC/VswellingUC.xlsx
+++ b/tests/materials/VSwellingUC/VswellingUC.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-11060" yWindow="-18000" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="solid" sheetId="1" r:id="rId1"/>
     <sheet name="gas" sheetId="2" r:id="rId2"/>
     <sheet name="densification" sheetId="3" r:id="rId3"/>
+    <sheet name="rz" sheetId="4" r:id="rId4"/>
+    <sheet name="constraint" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
   <si>
     <t>DV/v</t>
   </si>
@@ -144,19 +146,47 @@
   </si>
   <si>
     <t>3=</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> time           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> burnup         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> temp           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> volume         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> zone           </t>
+  </si>
+  <si>
+    <t>solid factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUCK vol    </t>
+  </si>
+  <si>
+    <t>disp_x</t>
+  </si>
+  <si>
+    <t>vol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="0.0000000000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0000E+00"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
     <numFmt numFmtId="168" formatCode="0.000000E+00"/>
     <numFmt numFmtId="169" formatCode="0.00000"/>
+    <numFmt numFmtId="173" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -208,7 +238,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="246">
+  <cellStyleXfs count="268">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -455,8 +485,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -468,8 +520,9 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="246">
+  <cellStyles count="268">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -592,6 +645,17 @@
     <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -714,6 +778,17 @@
     <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -2056,7 +2131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -2112,15 +2187,15 @@
         <v>1</v>
       </c>
       <c r="G8" s="7">
-        <f>$G$4*(1-EXP(-E8/$G$5))</f>
+        <f t="shared" ref="G8:G13" si="0">$G$4*(1-EXP(-E8/$G$5))</f>
         <v>0</v>
       </c>
       <c r="H8" s="7">
-        <f>(1+G8)</f>
+        <f t="shared" ref="H8:H13" si="1">(1+G8)</f>
         <v>1</v>
       </c>
       <c r="I8" s="7">
-        <f>ABS(F8-H8)/H8*100</f>
+        <f t="shared" ref="I8:I13" si="2">ABS(F8-H8)/H8*100</f>
         <v>0</v>
       </c>
     </row>
@@ -2138,15 +2213,15 @@
         <v>0.98449540000000002</v>
       </c>
       <c r="G9" s="7">
-        <f>$G$4*(1-EXP(-E9/$G$5))</f>
+        <f t="shared" si="0"/>
         <v>-1.550872761216435E-2</v>
       </c>
       <c r="H9" s="7">
-        <f>(1+G9)</f>
+        <f t="shared" si="1"/>
         <v>0.98449127238783563</v>
       </c>
       <c r="I9" s="7">
-        <f>ABS(F9-H9)/H9*100</f>
+        <f t="shared" si="2"/>
         <v>4.1926345922639255E-4</v>
       </c>
     </row>
@@ -2161,15 +2236,15 @@
         <v>0.97606199999999999</v>
       </c>
       <c r="G10" s="7">
-        <f>$G$4*(1-EXP(-E10/$G$5))</f>
+        <f t="shared" si="0"/>
         <v>-2.3943318984672553E-2</v>
       </c>
       <c r="H10" s="7">
-        <f>(1+G10)</f>
+        <f t="shared" si="1"/>
         <v>0.9760566810153275</v>
       </c>
       <c r="I10" s="7">
-        <f>ABS(F10-H10)/H10*100</f>
+        <f t="shared" si="2"/>
         <v>5.4494629010208746E-4</v>
       </c>
     </row>
@@ -2184,15 +2259,15 @@
         <v>0.97147510000000004</v>
       </c>
       <c r="G11" s="7">
-        <f>$G$4*(1-EXP(-E11/$G$5))</f>
+        <f t="shared" si="0"/>
         <v>-2.8530563883176607E-2</v>
       </c>
       <c r="H11" s="7">
-        <f>(1+G11)</f>
+        <f t="shared" si="1"/>
         <v>0.97146943611682335</v>
       </c>
       <c r="I11" s="7">
-        <f>ABS(F11-H11)/H11*100</f>
+        <f t="shared" si="2"/>
         <v>5.8302227184082274E-4</v>
       </c>
     </row>
@@ -2207,15 +2282,15 @@
         <v>0.96898039999999996</v>
       </c>
       <c r="G12" s="7">
-        <f>$G$4*(1-EXP(-E12/$G$5))</f>
+        <f t="shared" si="0"/>
         <v>-3.1025387263410368E-2</v>
       </c>
       <c r="H12" s="7">
-        <f>(1+G12)</f>
+        <f t="shared" si="1"/>
         <v>0.96897461273658958</v>
       </c>
       <c r="I12" s="7">
-        <f>ABS(F12-H12)/H12*100</f>
+        <f t="shared" si="2"/>
         <v>5.9725645381352962E-4</v>
       </c>
     </row>
@@ -2230,15 +2305,15 @@
         <v>0.96762360000000003</v>
       </c>
       <c r="G13" s="7">
-        <f>$G$4*(1-EXP(-E13/$G$5))</f>
+        <f t="shared" si="0"/>
         <v>-3.2382224283511646E-2</v>
       </c>
       <c r="H13" s="7">
-        <f>(1+G13)</f>
+        <f t="shared" si="1"/>
         <v>0.96761777571648833</v>
       </c>
       <c r="I13" s="7">
-        <f>ABS(F13-H13)/H13*100</f>
+        <f t="shared" si="2"/>
         <v>6.0191985491265252E-4</v>
       </c>
     </row>
@@ -2297,4 +2372,575 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E5:K29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20:J27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="5:11">
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="5:11">
+      <c r="E9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="5:11">
+      <c r="E10" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3.6543699999999998E-2</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1130</v>
+      </c>
+      <c r="H10" s="8">
+        <v>3.198995</v>
+      </c>
+      <c r="I10" s="3">
+        <v>4</v>
+      </c>
+      <c r="J10" s="8">
+        <f>($G$5*F10+1)*PI()</f>
+        <v>3.1989953633172878</v>
+      </c>
+      <c r="K10">
+        <f>ABS(J10-H10)/J10*100</f>
+        <v>1.1357230834920895E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="5:11">
+      <c r="E11" s="3">
+        <v>20000000</v>
+      </c>
+      <c r="F11" s="3">
+        <v>7.3087399999999997E-2</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1130</v>
+      </c>
+      <c r="H11" s="8">
+        <v>3.2563979999999999</v>
+      </c>
+      <c r="I11" s="3">
+        <v>4</v>
+      </c>
+      <c r="J11" s="8">
+        <f t="shared" ref="J11:J16" si="0">($G$5*F11+1)*PI()</f>
+        <v>3.2563980730447821</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ref="K11:K16" si="1">ABS(J11-H11)/J11*100</f>
+        <v>2.2431158778604314E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="5:11">
+      <c r="E12" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.1096311</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1130</v>
+      </c>
+      <c r="H12" s="8">
+        <v>3.3138010000000002</v>
+      </c>
+      <c r="I12" s="3">
+        <v>3</v>
+      </c>
+      <c r="J12" s="8">
+        <f t="shared" si="0"/>
+        <v>3.3138007827722773</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>6.555243877362017E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="5:11">
+      <c r="E13" s="3">
+        <v>40000000</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.14617479999999999</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1130</v>
+      </c>
+      <c r="H13" s="8">
+        <v>3.3712029999999999</v>
+      </c>
+      <c r="I13" s="3">
+        <v>3</v>
+      </c>
+      <c r="J13" s="8">
+        <f t="shared" si="0"/>
+        <v>3.3712034924997716</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>1.4609019382166677E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="5:11">
+      <c r="E14" s="3">
+        <v>50000000</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.18271850000000001</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1130</v>
+      </c>
+      <c r="H14" s="8">
+        <v>3.4286059999999998</v>
+      </c>
+      <c r="I14" s="3">
+        <v>3</v>
+      </c>
+      <c r="J14" s="8">
+        <f t="shared" si="0"/>
+        <v>3.4286062022272663</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>5.8982354508003633E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="5:11">
+      <c r="E15" s="3">
+        <v>60000000</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.21926219999999999</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1130</v>
+      </c>
+      <c r="H15" s="8">
+        <v>3.4860090000000001</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1</v>
+      </c>
+      <c r="J15" s="8">
+        <f t="shared" si="0"/>
+        <v>3.4860089119547615</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>2.5256745142967342E-6</v>
+      </c>
+    </row>
+    <row r="16" spans="5:11">
+      <c r="E16" s="3">
+        <v>70000000</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.25580589999999997</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1130</v>
+      </c>
+      <c r="H16" s="8">
+        <v>3.543412</v>
+      </c>
+      <c r="I16" s="3">
+        <v>1</v>
+      </c>
+      <c r="J16" s="8">
+        <f t="shared" si="0"/>
+        <v>3.5434116216822558</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>1.0676652464759312E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="5:10">
+      <c r="H17" s="8"/>
+    </row>
+    <row r="20" spans="5:10">
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="5:10">
+      <c r="E21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="6">
+        <v>10</v>
+      </c>
+      <c r="G21" s="10">
+        <v>3.6543699999999998E-2</v>
+      </c>
+      <c r="H21" s="8">
+        <v>3.198995</v>
+      </c>
+      <c r="I21" s="11">
+        <v>3.1989953633172878</v>
+      </c>
+      <c r="J21">
+        <v>1.1357230834920895E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="5:10">
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="6">
+        <v>20</v>
+      </c>
+      <c r="G22" s="10">
+        <v>7.3087399999999997E-2</v>
+      </c>
+      <c r="H22" s="8">
+        <v>3.2563979999999999</v>
+      </c>
+      <c r="I22" s="11">
+        <v>3.2563980730447821</v>
+      </c>
+      <c r="J22">
+        <v>2.2431158778604314E-6</v>
+      </c>
+    </row>
+    <row r="23" spans="5:10">
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="6">
+        <v>30</v>
+      </c>
+      <c r="G23" s="10">
+        <v>0.1096311</v>
+      </c>
+      <c r="H23" s="8">
+        <v>3.3138010000000002</v>
+      </c>
+      <c r="I23" s="11">
+        <v>3.3138007827722773</v>
+      </c>
+      <c r="J23">
+        <v>6.555243877362017E-6</v>
+      </c>
+    </row>
+    <row r="24" spans="5:10">
+      <c r="E24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="6">
+        <v>40</v>
+      </c>
+      <c r="G24" s="10">
+        <v>0.14617479999999999</v>
+      </c>
+      <c r="H24" s="8">
+        <v>3.3712029999999999</v>
+      </c>
+      <c r="I24" s="11">
+        <v>3.3712034924997716</v>
+      </c>
+      <c r="J24">
+        <v>1.4609019382166677E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="5:10">
+      <c r="E25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="6">
+        <v>50</v>
+      </c>
+      <c r="G25" s="10">
+        <v>0.18271850000000001</v>
+      </c>
+      <c r="H25" s="8">
+        <v>3.4286059999999998</v>
+      </c>
+      <c r="I25" s="11">
+        <v>3.4286062022272663</v>
+      </c>
+      <c r="J25">
+        <v>5.8982354508003633E-6</v>
+      </c>
+    </row>
+    <row r="26" spans="5:10">
+      <c r="E26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="6">
+        <v>60</v>
+      </c>
+      <c r="G26" s="10">
+        <v>0.21926219999999999</v>
+      </c>
+      <c r="H26" s="8">
+        <v>3.4860090000000001</v>
+      </c>
+      <c r="I26" s="11">
+        <v>3.4860089119547615</v>
+      </c>
+      <c r="J26">
+        <v>2.5256745142967342E-6</v>
+      </c>
+    </row>
+    <row r="27" spans="5:10">
+      <c r="E27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="6">
+        <v>70</v>
+      </c>
+      <c r="G27" s="10">
+        <v>0.25580589999999997</v>
+      </c>
+      <c r="H27" s="8">
+        <v>3.543412</v>
+      </c>
+      <c r="I27" s="11">
+        <v>3.5434116216822558</v>
+      </c>
+      <c r="J27">
+        <v>1.0676652464759312E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="5:10">
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="5:10">
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C9:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="9" spans="3:8">
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8">
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="6">
+        <v>10</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="H10" s="8">
+        <f>(1-F10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8">
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="6">
+        <v>20</v>
+      </c>
+      <c r="E11" s="8">
+        <v>3.6543699999999998E-2</v>
+      </c>
+      <c r="F11" s="8">
+        <v>-1.128727E-2</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1.011287</v>
+      </c>
+      <c r="H11" s="8">
+        <f t="shared" ref="H11:H15" si="0">(1-F11)</f>
+        <v>1.01128727</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8">
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="6">
+        <v>30</v>
+      </c>
+      <c r="E12" s="8">
+        <v>7.3087399999999997E-2</v>
+      </c>
+      <c r="F12" s="8">
+        <v>-2.2523390000000001E-2</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1.0225230000000001</v>
+      </c>
+      <c r="H12" s="8">
+        <f t="shared" si="0"/>
+        <v>1.0225233899999999</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8">
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="6">
+        <v>40</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.1096311</v>
+      </c>
+      <c r="F13" s="8">
+        <v>-3.3709669999999997E-2</v>
+      </c>
+      <c r="G13" s="8">
+        <v>1.0337099999999999</v>
+      </c>
+      <c r="H13" s="8">
+        <f t="shared" si="0"/>
+        <v>1.0337096699999999</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8">
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="6">
+        <v>50</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.14617479999999999</v>
+      </c>
+      <c r="F14" s="8">
+        <v>-4.4847360000000003E-2</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1.0448470000000001</v>
+      </c>
+      <c r="H14" s="8">
+        <f t="shared" si="0"/>
+        <v>1.0448473599999999</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8">
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="6">
+        <v>60</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0.18271850000000001</v>
+      </c>
+      <c r="F15" s="8">
+        <v>-5.5937670000000002E-2</v>
+      </c>
+      <c r="G15" s="8">
+        <v>1.055938</v>
+      </c>
+      <c r="H15" s="8">
+        <f t="shared" si="0"/>
+        <v>1.0559376700000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added flag to allow central swelling
</commit_message>
<xml_diff>
--- a/tests/materials/VSwellingUC/VswellingUC.xlsx
+++ b/tests/materials/VSwellingUC/VswellingUC.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
   <si>
     <t>DV/v</t>
   </si>
@@ -170,9 +170,6 @@
   </si>
   <si>
     <t>disp_x</t>
-  </si>
-  <si>
-    <t>vol</t>
   </si>
 </sst>
 </file>
@@ -238,9 +235,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="268">
+  <cellStyleXfs count="270">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -522,7 +521,7 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="268">
+  <cellStyles count="270">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -656,6 +655,7 @@
     <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -789,6 +789,7 @@
     <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -2784,7 +2785,7 @@
   <dimension ref="C9:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C15"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2803,7 +2804,7 @@
         <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="H9" t="s">
         <v>38</v>
@@ -2937,6 +2938,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>